<commit_message>
Indigenous hild mortality text fixes May31#14
</commit_message>
<xml_diff>
--- a/dashboard_loader/indigenous_child_mortality_uploader/indigenous_child_mortality.xlsx
+++ b/dashboard_loader/indigenous_child_mortality_uploader/indigenous_child_mortality.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -126,7 +126,7 @@
     <t xml:space="preserve">Desc Body</t>
   </si>
   <si>
-    <t xml:space="preserve">This target is on track this year. The 2016 Indigenous child mortality rate has returned to being within the range required for this target to be on track. Over the long-term (1998 to 2016), the Indigenous child mortality rate declined significantly (by 35 per cent). There was also a significant narrowing (32 per cent) of the child mortality gap. In the short-term, the decline in Indigenous child mortality rates between 2008 and 2016 was not statistically significant.</t>
+    <t xml:space="preserve">This target is on track this year. The 2016 Indigenous child mortality rate has returned to being within the range required for this target to be on track. Over the long-term (1998 to 2016), the Indigenous child mortality rate declined significantly (by 35 per cent). There was also a significant narrowing (32 per cent) of the child mortality gap. The decline in Indigenous child mortality rates between 2008 (the baseline year) and 2016 was not statistically significant.</t>
   </si>
   <si>
     <t xml:space="preserve">State and Territory child mortality rates by Indigenous status for the period 2012 to 2016 show there is some variation by geography. New South Wales had the lowest Indigenous child mortality rate (110 child deaths per 100,000 population) and the smallest gap compared with non-Indigenous children. The Northern Territory had the highest Indigenous child mortality rate (332 child deaths per 100,000 population) and the largest absolute gap.</t>
@@ -1512,7 +1512,7 @@
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -1750,8 +1750,8 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1793,7 +1793,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="66" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>32</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>36</v>
       </c>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="D8" s="13"/>
     </row>
-    <row r="9" customFormat="false" ht="62.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
       <c r="B9" s="14" t="s">
         <v>38</v>

</xml_diff>